<commit_message>
Sanity check for the day updated
</commit_message>
<xml_diff>
--- a/eclipse-workspace/TestNG1/TestData/ExcelAuto.xlsx
+++ b/eclipse-workspace/TestNG1/TestData/ExcelAuto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swathi\eclipse-workspace\TestNG1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A658A9-1E90-46F7-BA33-663D4DFE4331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440A275E-E3D8-4467-AA10-BF6C56FA86DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3726E1BC-A6BE-4FB2-8055-91D1E7B04C72}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>"12345"</t>
   </si>
   <si>
-    <t>rahul</t>
+    <t>chidambaram</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Last commit for the day
</commit_message>
<xml_diff>
--- a/eclipse-workspace/TestNG1/TestData/ExcelAuto.xlsx
+++ b/eclipse-workspace/TestNG1/TestData/ExcelAuto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swathi\eclipse-workspace\TestNG1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440A275E-E3D8-4467-AA10-BF6C56FA86DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B45DA5A-2D2D-4114-842A-B41C234BCE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3726E1BC-A6BE-4FB2-8055-91D1E7B04C72}"/>
   </bookViews>
@@ -60,10 +60,10 @@
     <t>swathi</t>
   </si>
   <si>
-    <t>"12345"</t>
-  </si>
-  <si>
     <t>chidambaram</t>
+  </si>
+  <si>
+    <t>"1234567"</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -455,10 +455,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>